<commit_message>
Create lookupgenerator and fix some inputs
</commit_message>
<xml_diff>
--- a/input_xlsx/Hassan 005.xlsx
+++ b/input_xlsx/Hassan 005.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Biodiverskripsi\Papua\Skripsi &amp; Transkripsi\Hassan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\PROJECTS\biodiverskripsi_data_visualization\input_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A4E59C-87E7-4472-899F-F05438CBB88E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FE1A94-0103-4262-91DB-76E21053C74E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Events" sheetId="2" r:id="rId1"/>
@@ -2471,7 +2471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
   <si>
     <t>occurrenceID</t>
   </si>
@@ -2636,12 +2636,6 @@
   </si>
   <si>
     <t>2002-04-04/2002-04-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analisis data dilakukan secara statistik.  Statistik deskriptif secara tabulasi </t>
-  </si>
-  <si>
-    <t>digunakan untuk melihat produksi kayu bulat PT. Prabu Alaska Unit I</t>
   </si>
   <si>
     <t>Vegetasi</t>
@@ -2833,6 +2827,9 @@
   </si>
   <si>
     <t>Skripsi Ini Milik universitas Papua</t>
+  </si>
+  <si>
+    <t>Analisis data dilakukan secara statistik.  Statistik deskriptif secara tabulasi digunakan untuk melihat produksi kayu bulat PT. Prabu Alaska Unit I</t>
   </si>
 </sst>
 </file>
@@ -3566,9 +3563,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3667,22 +3664,22 @@
         <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
         <v>51</v>
       </c>
       <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>59</v>
-      </c>
       <c r="L2" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M2" t="s">
         <v>46</v>
@@ -3697,22 +3694,20 @@
         <v>48</v>
       </c>
       <c r="Q2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E3"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
     </row>
@@ -3825,7 +3820,7 @@
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -3837,16 +3832,16 @@
         <v>49</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>50</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s">
         <v>46</v>
@@ -3861,7 +3856,7 @@
         <v>54</v>
       </c>
       <c r="Q2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -3869,7 +3864,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
@@ -3881,16 +3876,16 @@
         <v>49</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
         <v>50</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K3" t="s">
         <v>46</v>
@@ -3905,7 +3900,7 @@
         <v>54</v>
       </c>
       <c r="Q3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -3913,7 +3908,7 @@
         <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
@@ -3925,16 +3920,16 @@
         <v>49</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G4" t="s">
         <v>50</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
         <v>46</v>
@@ -3949,7 +3944,7 @@
         <v>54</v>
       </c>
       <c r="Q4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3957,7 +3952,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
@@ -3969,16 +3964,16 @@
         <v>49</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
         <v>50</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K5" t="s">
         <v>46</v>
@@ -3993,7 +3988,7 @@
         <v>54</v>
       </c>
       <c r="Q5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -4001,7 +3996,7 @@
         <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
         <v>44</v>
@@ -4013,16 +4008,16 @@
         <v>49</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
         <v>52</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K6" t="s">
         <v>46</v>
@@ -4037,7 +4032,7 @@
         <v>54</v>
       </c>
       <c r="Q6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -4203,28 +4198,28 @@
         <v>53</v>
       </c>
       <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" t="s">
-        <v>80</v>
       </c>
       <c r="F2" t="s">
         <v>54</v>
       </c>
       <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" t="s">
         <v>81</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="I2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>